<commit_message>
NHS report - Began to use ChatGPT
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/31f71df29d48a75f/Documents/GitHub/NHS-report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/31f71df29d48a75f/Documents/GitHub/NHS-report/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="8_{2ABBD5E6-42EC-4661-89A9-0942CB396BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA64668E-E5E7-48DC-BEE6-652754218EB1}"/>
+  <xr:revisionPtr revIDLastSave="145" documentId="8_{2ABBD5E6-42EC-4661-89A9-0942CB396BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{893A6D2D-4EF4-4E03-90FA-C874634DB666}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{39AE5F7D-C74D-4C47-9EAD-B955BBC20FF6}"/>
   </bookViews>
@@ -39,60 +39,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="546">
   <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>numeric1</t>
-  </si>
-  <si>
-    <t>verbal1</t>
-  </si>
-  <si>
-    <t>induct1</t>
-  </si>
-  <si>
-    <t>numeric2</t>
-  </si>
-  <si>
-    <t>verbal2</t>
-  </si>
-  <si>
-    <t>induct2</t>
-  </si>
-  <si>
-    <t>numeric3</t>
-  </si>
-  <si>
-    <t>verbal3</t>
-  </si>
-  <si>
-    <t>induct3</t>
-  </si>
-  <si>
-    <t>numeric4</t>
-  </si>
-  <si>
-    <t>verbal4</t>
-  </si>
-  <si>
-    <t>induct4</t>
-  </si>
-  <si>
-    <t>numeric5</t>
-  </si>
-  <si>
-    <t>verbal5</t>
-  </si>
-  <si>
-    <t>induct5</t>
-  </si>
-  <si>
-    <t>numeric6</t>
-  </si>
-  <si>
-    <t>verbal6</t>
-  </si>
-  <si>
-    <t>induct6</t>
   </si>
   <si>
     <t>fdt_activ</t>
@@ -1675,6 +1621,60 @@
   <si>
     <t>participant500</t>
   </si>
+  <si>
+    <t>cog_num_1</t>
+  </si>
+  <si>
+    <t>cog_num_2</t>
+  </si>
+  <si>
+    <t>cog_num_3</t>
+  </si>
+  <si>
+    <t>cog_num_4</t>
+  </si>
+  <si>
+    <t>cog_num_5</t>
+  </si>
+  <si>
+    <t>cog_num_6</t>
+  </si>
+  <si>
+    <t>cog_ver_1</t>
+  </si>
+  <si>
+    <t>cog_ver_2</t>
+  </si>
+  <si>
+    <t>cog_ver_3</t>
+  </si>
+  <si>
+    <t>cog_ver_4</t>
+  </si>
+  <si>
+    <t>cog_ver_5</t>
+  </si>
+  <si>
+    <t>cog_ver_6</t>
+  </si>
+  <si>
+    <t>cog_abs_1</t>
+  </si>
+  <si>
+    <t>cog_abs_2</t>
+  </si>
+  <si>
+    <t>cog_abs_3</t>
+  </si>
+  <si>
+    <t>cog_abs_4</t>
+  </si>
+  <si>
+    <t>cog_abs_5</t>
+  </si>
+  <si>
+    <t>cog_abs_6</t>
+  </si>
 </sst>
 </file>
 
@@ -1732,6 +1732,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2034,7 +2038,7 @@
   <dimension ref="A1:AT501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2047,144 +2051,144 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>528</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>529</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>530</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>531</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>532</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>533</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>534</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>535</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>536</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>537</v>
       </c>
       <c r="L1" t="s">
+        <v>538</v>
+      </c>
+      <c r="M1" t="s">
+        <v>539</v>
+      </c>
+      <c r="N1" t="s">
+        <v>540</v>
+      </c>
+      <c r="O1" t="s">
+        <v>541</v>
+      </c>
+      <c r="P1" t="s">
+        <v>542</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>543</v>
+      </c>
+      <c r="R1" t="s">
+        <v>544</v>
+      </c>
+      <c r="S1" t="s">
+        <v>545</v>
+      </c>
+      <c r="T1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" t="s">
+        <v>3</v>
+      </c>
+      <c r="X1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="AH1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AJ1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AK1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="AL1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AM1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>44</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="AP1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AQ1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AR1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AS1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA1" t="s">
+      <c r="AT1" t="s">
         <v>25</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -2324,7 +2328,7 @@
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -2464,7 +2468,7 @@
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -2604,7 +2608,7 @@
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>8</v>
@@ -2744,7 +2748,7 @@
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -2884,7 +2888,7 @@
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B7">
         <v>7</v>
@@ -3024,7 +3028,7 @@
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>9</v>
@@ -3164,7 +3168,7 @@
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B9">
         <v>10</v>
@@ -3304,7 +3308,7 @@
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -3444,7 +3448,7 @@
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -3584,7 +3588,7 @@
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -3724,7 +3728,7 @@
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -3864,7 +3868,7 @@
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -4004,7 +4008,7 @@
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -4144,7 +4148,7 @@
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -4284,7 +4288,7 @@
     </row>
     <row r="17" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -4424,7 +4428,7 @@
     </row>
     <row r="18" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -4564,7 +4568,7 @@
     </row>
     <row r="19" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B19">
         <v>8</v>
@@ -4704,7 +4708,7 @@
     </row>
     <row r="20" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="B20">
         <v>5</v>
@@ -4844,7 +4848,7 @@
     </row>
     <row r="21" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -4984,7 +4988,7 @@
     </row>
     <row r="22" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="B22">
         <v>7</v>
@@ -5124,7 +5128,7 @@
     </row>
     <row r="23" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="B23">
         <v>10</v>
@@ -5264,7 +5268,7 @@
     </row>
     <row r="24" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -5404,7 +5408,7 @@
     </row>
     <row r="25" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B25">
         <v>7</v>
@@ -5544,7 +5548,7 @@
     </row>
     <row r="26" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="B26">
         <v>8</v>
@@ -5684,7 +5688,7 @@
     </row>
     <row r="27" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -5824,7 +5828,7 @@
     </row>
     <row r="28" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="B28">
         <v>6</v>
@@ -5964,7 +5968,7 @@
     </row>
     <row r="29" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="B29">
         <v>9</v>
@@ -6104,7 +6108,7 @@
     </row>
     <row r="30" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="B30">
         <v>7</v>
@@ -6244,7 +6248,7 @@
     </row>
     <row r="31" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B31">
         <v>4</v>
@@ -6384,7 +6388,7 @@
     </row>
     <row r="32" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="B32">
         <v>8</v>
@@ -6524,7 +6528,7 @@
     </row>
     <row r="33" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="B33">
         <v>8</v>
@@ -6664,7 +6668,7 @@
     </row>
     <row r="34" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="B34">
         <v>6</v>
@@ -6804,7 +6808,7 @@
     </row>
     <row r="35" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="B35">
         <v>5</v>
@@ -6944,7 +6948,7 @@
     </row>
     <row r="36" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B36">
         <v>7</v>
@@ -7084,7 +7088,7 @@
     </row>
     <row r="37" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="B37">
         <v>4</v>
@@ -7224,7 +7228,7 @@
     </row>
     <row r="38" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="B38">
         <v>8</v>
@@ -7364,7 +7368,7 @@
     </row>
     <row r="39" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="B39">
         <v>3</v>
@@ -7504,7 +7508,7 @@
     </row>
     <row r="40" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B40">
         <v>9</v>
@@ -7644,7 +7648,7 @@
     </row>
     <row r="41" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="B41">
         <v>10</v>
@@ -7784,7 +7788,7 @@
     </row>
     <row r="42" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -7924,7 +7928,7 @@
     </row>
     <row r="43" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="B43">
         <v>8</v>
@@ -8064,7 +8068,7 @@
     </row>
     <row r="44" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B44">
         <v>7</v>
@@ -8204,7 +8208,7 @@
     </row>
     <row r="45" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="B45">
         <v>6</v>
@@ -8344,7 +8348,7 @@
     </row>
     <row r="46" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="B46">
         <v>7</v>
@@ -8484,7 +8488,7 @@
     </row>
     <row r="47" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="B47">
         <v>3</v>
@@ -8624,7 +8628,7 @@
     </row>
     <row r="48" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="B48">
         <v>8</v>
@@ -8764,7 +8768,7 @@
     </row>
     <row r="49" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="B49">
         <v>4</v>
@@ -8904,7 +8908,7 @@
     </row>
     <row r="50" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="B50">
         <v>10</v>
@@ -9044,7 +9048,7 @@
     </row>
     <row r="51" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="B51">
         <v>7</v>
@@ -9184,7 +9188,7 @@
     </row>
     <row r="52" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="B52">
         <v>5</v>
@@ -9324,7 +9328,7 @@
     </row>
     <row r="53" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="B53">
         <v>2</v>
@@ -9464,7 +9468,7 @@
     </row>
     <row r="54" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="B54">
         <v>10</v>
@@ -9604,7 +9608,7 @@
     </row>
     <row r="55" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="B55">
         <v>5</v>
@@ -9744,7 +9748,7 @@
     </row>
     <row r="56" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="B56">
         <v>9</v>
@@ -9884,7 +9888,7 @@
     </row>
     <row r="57" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="B57">
         <v>9</v>
@@ -10024,7 +10028,7 @@
     </row>
     <row r="58" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B58">
         <v>8</v>
@@ -10164,7 +10168,7 @@
     </row>
     <row r="59" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="B59">
         <v>4</v>
@@ -10304,7 +10308,7 @@
     </row>
     <row r="60" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="B60">
         <v>6</v>
@@ -10444,7 +10448,7 @@
     </row>
     <row r="61" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="B61">
         <v>5</v>
@@ -10584,7 +10588,7 @@
     </row>
     <row r="62" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="B62">
         <v>10</v>
@@ -10724,7 +10728,7 @@
     </row>
     <row r="63" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="B63">
         <v>5</v>
@@ -10864,7 +10868,7 @@
     </row>
     <row r="64" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="B64">
         <v>6</v>
@@ -11004,7 +11008,7 @@
     </row>
     <row r="65" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -11144,7 +11148,7 @@
     </row>
     <row r="66" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="B66">
         <v>5</v>
@@ -11284,7 +11288,7 @@
     </row>
     <row r="67" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="B67">
         <v>9</v>
@@ -11424,7 +11428,7 @@
     </row>
     <row r="68" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="B68">
         <v>4</v>
@@ -11564,7 +11568,7 @@
     </row>
     <row r="69" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="B69">
         <v>8</v>
@@ -11704,7 +11708,7 @@
     </row>
     <row r="70" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="B70">
         <v>5</v>
@@ -11844,7 +11848,7 @@
     </row>
     <row r="71" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -11984,7 +11988,7 @@
     </row>
     <row r="72" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="B72">
         <v>6</v>
@@ -12124,7 +12128,7 @@
     </row>
     <row r="73" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="B73">
         <v>10</v>
@@ -12264,7 +12268,7 @@
     </row>
     <row r="74" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="B74">
         <v>9</v>
@@ -12404,7 +12408,7 @@
     </row>
     <row r="75" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="B75">
         <v>8</v>
@@ -12544,7 +12548,7 @@
     </row>
     <row r="76" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="B76">
         <v>3</v>
@@ -12684,7 +12688,7 @@
     </row>
     <row r="77" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="B77">
         <v>7</v>
@@ -12824,7 +12828,7 @@
     </row>
     <row r="78" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -12964,7 +12968,7 @@
     </row>
     <row r="79" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="B79">
         <v>2</v>
@@ -13104,7 +13108,7 @@
     </row>
     <row r="80" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="B80">
         <v>3</v>
@@ -13244,7 +13248,7 @@
     </row>
     <row r="81" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="B81">
         <v>7</v>
@@ -13384,7 +13388,7 @@
     </row>
     <row r="82" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="B82">
         <v>9</v>
@@ -13524,7 +13528,7 @@
     </row>
     <row r="83" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B83">
         <v>7</v>
@@ -13664,7 +13668,7 @@
     </row>
     <row r="84" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="B84">
         <v>5</v>
@@ -13804,7 +13808,7 @@
     </row>
     <row r="85" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="B85">
         <v>4</v>
@@ -13944,7 +13948,7 @@
     </row>
     <row r="86" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="B86">
         <v>9</v>
@@ -14084,7 +14088,7 @@
     </row>
     <row r="87" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -14224,7 +14228,7 @@
     </row>
     <row r="88" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="B88">
         <v>5</v>
@@ -14364,7 +14368,7 @@
     </row>
     <row r="89" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="B89">
         <v>5</v>
@@ -14504,7 +14508,7 @@
     </row>
     <row r="90" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="B90">
         <v>8</v>
@@ -14644,7 +14648,7 @@
     </row>
     <row r="91" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="B91">
         <v>10</v>
@@ -14784,7 +14788,7 @@
     </row>
     <row r="92" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -14924,7 +14928,7 @@
     </row>
     <row r="93" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="B93">
         <v>6</v>
@@ -15064,7 +15068,7 @@
     </row>
     <row r="94" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="B94">
         <v>2</v>
@@ -15204,7 +15208,7 @@
     </row>
     <row r="95" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="B95">
         <v>2</v>
@@ -15344,7 +15348,7 @@
     </row>
     <row r="96" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="B96">
         <v>8</v>
@@ -15484,7 +15488,7 @@
     </row>
     <row r="97" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="B97">
         <v>4</v>
@@ -15624,7 +15628,7 @@
     </row>
     <row r="98" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="B98">
         <v>6</v>
@@ -15764,7 +15768,7 @@
     </row>
     <row r="99" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="B99">
         <v>8</v>
@@ -15904,7 +15908,7 @@
     </row>
     <row r="100" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="B100">
         <v>6</v>
@@ -16044,7 +16048,7 @@
     </row>
     <row r="101" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="B101">
         <v>6</v>
@@ -16184,7 +16188,7 @@
     </row>
     <row r="102" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="B102">
         <v>9</v>
@@ -16324,7 +16328,7 @@
     </row>
     <row r="103" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B103">
         <v>6</v>
@@ -16464,7 +16468,7 @@
     </row>
     <row r="104" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="B104">
         <v>6</v>
@@ -16604,7 +16608,7 @@
     </row>
     <row r="105" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="B105">
         <v>4</v>
@@ -16744,7 +16748,7 @@
     </row>
     <row r="106" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="B106">
         <v>6</v>
@@ -16884,7 +16888,7 @@
     </row>
     <row r="107" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="B107">
         <v>7</v>
@@ -17024,7 +17028,7 @@
     </row>
     <row r="108" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="B108">
         <v>4</v>
@@ -17164,7 +17168,7 @@
     </row>
     <row r="109" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="B109">
         <v>4</v>
@@ -17304,7 +17308,7 @@
     </row>
     <row r="110" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="B110">
         <v>2</v>
@@ -17444,7 +17448,7 @@
     </row>
     <row r="111" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B111">
         <v>7</v>
@@ -17584,7 +17588,7 @@
     </row>
     <row r="112" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="B112">
         <v>2</v>
@@ -17724,7 +17728,7 @@
     </row>
     <row r="113" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="B113">
         <v>5</v>
@@ -17864,7 +17868,7 @@
     </row>
     <row r="114" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="B114">
         <v>2</v>
@@ -18004,7 +18008,7 @@
     </row>
     <row r="115" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="B115">
         <v>4</v>
@@ -18144,7 +18148,7 @@
     </row>
     <row r="116" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="B116">
         <v>4</v>
@@ -18284,7 +18288,7 @@
     </row>
     <row r="117" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="B117">
         <v>1</v>
@@ -18424,7 +18428,7 @@
     </row>
     <row r="118" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="B118">
         <v>1</v>
@@ -18564,7 +18568,7 @@
     </row>
     <row r="119" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="B119">
         <v>5</v>
@@ -18704,7 +18708,7 @@
     </row>
     <row r="120" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="B120">
         <v>10</v>
@@ -18844,7 +18848,7 @@
     </row>
     <row r="121" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="B121">
         <v>10</v>
@@ -18984,7 +18988,7 @@
     </row>
     <row r="122" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="B122">
         <v>2</v>
@@ -19124,7 +19128,7 @@
     </row>
     <row r="123" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="B123">
         <v>10</v>
@@ -19264,7 +19268,7 @@
     </row>
     <row r="124" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="B124">
         <v>4</v>
@@ -19404,7 +19408,7 @@
     </row>
     <row r="125" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="B125">
         <v>10</v>
@@ -19544,7 +19548,7 @@
     </row>
     <row r="126" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="B126">
         <v>10</v>
@@ -19684,7 +19688,7 @@
     </row>
     <row r="127" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="B127">
         <v>5</v>
@@ -19824,7 +19828,7 @@
     </row>
     <row r="128" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="B128">
         <v>8</v>
@@ -19964,7 +19968,7 @@
     </row>
     <row r="129" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="B129">
         <v>7</v>
@@ -20104,7 +20108,7 @@
     </row>
     <row r="130" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="B130">
         <v>10</v>
@@ -20244,7 +20248,7 @@
     </row>
     <row r="131" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="B131">
         <v>1</v>
@@ -20384,7 +20388,7 @@
     </row>
     <row r="132" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="B132">
         <v>1</v>
@@ -20524,7 +20528,7 @@
     </row>
     <row r="133" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="B133">
         <v>7</v>
@@ -20664,7 +20668,7 @@
     </row>
     <row r="134" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="B134">
         <v>1</v>
@@ -20804,7 +20808,7 @@
     </row>
     <row r="135" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="B135">
         <v>2</v>
@@ -20944,7 +20948,7 @@
     </row>
     <row r="136" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="B136">
         <v>10</v>
@@ -21084,7 +21088,7 @@
     </row>
     <row r="137" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="B137">
         <v>9</v>
@@ -21224,7 +21228,7 @@
     </row>
     <row r="138" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="B138">
         <v>4</v>
@@ -21364,7 +21368,7 @@
     </row>
     <row r="139" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="B139">
         <v>1</v>
@@ -21504,7 +21508,7 @@
     </row>
     <row r="140" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="B140">
         <v>5</v>
@@ -21644,7 +21648,7 @@
     </row>
     <row r="141" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="B141">
         <v>6</v>
@@ -21784,7 +21788,7 @@
     </row>
     <row r="142" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="B142">
         <v>10</v>
@@ -21924,7 +21928,7 @@
     </row>
     <row r="143" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="B143">
         <v>10</v>
@@ -22064,7 +22068,7 @@
     </row>
     <row r="144" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="B144">
         <v>1</v>
@@ -22204,7 +22208,7 @@
     </row>
     <row r="145" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="B145">
         <v>7</v>
@@ -22344,7 +22348,7 @@
     </row>
     <row r="146" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="B146">
         <v>9</v>
@@ -22484,7 +22488,7 @@
     </row>
     <row r="147" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="B147">
         <v>3</v>
@@ -22624,7 +22628,7 @@
     </row>
     <row r="148" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="B148">
         <v>1</v>
@@ -22764,7 +22768,7 @@
     </row>
     <row r="149" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="B149">
         <v>2</v>
@@ -22904,7 +22908,7 @@
     </row>
     <row r="150" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="B150">
         <v>6</v>
@@ -23044,7 +23048,7 @@
     </row>
     <row r="151" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="B151">
         <v>2</v>
@@ -23184,7 +23188,7 @@
     </row>
     <row r="152" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="B152">
         <v>7</v>
@@ -23324,7 +23328,7 @@
     </row>
     <row r="153" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="B153">
         <v>8</v>
@@ -23464,7 +23468,7 @@
     </row>
     <row r="154" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="B154">
         <v>8</v>
@@ -23604,7 +23608,7 @@
     </row>
     <row r="155" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="B155">
         <v>9</v>
@@ -23744,7 +23748,7 @@
     </row>
     <row r="156" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="B156">
         <v>3</v>
@@ -23884,7 +23888,7 @@
     </row>
     <row r="157" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="B157">
         <v>1</v>
@@ -24024,7 +24028,7 @@
     </row>
     <row r="158" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="B158">
         <v>10</v>
@@ -24164,7 +24168,7 @@
     </row>
     <row r="159" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="B159">
         <v>8</v>
@@ -24304,7 +24308,7 @@
     </row>
     <row r="160" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="B160">
         <v>4</v>
@@ -24444,7 +24448,7 @@
     </row>
     <row r="161" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="B161">
         <v>1</v>
@@ -24584,7 +24588,7 @@
     </row>
     <row r="162" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="B162">
         <v>6</v>
@@ -24724,7 +24728,7 @@
     </row>
     <row r="163" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="B163">
         <v>4</v>
@@ -24864,7 +24868,7 @@
     </row>
     <row r="164" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="B164">
         <v>10</v>
@@ -25004,7 +25008,7 @@
     </row>
     <row r="165" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="B165">
         <v>8</v>
@@ -25144,7 +25148,7 @@
     </row>
     <row r="166" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="B166">
         <v>6</v>
@@ -25284,7 +25288,7 @@
     </row>
     <row r="167" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="B167">
         <v>9</v>
@@ -25424,7 +25428,7 @@
     </row>
     <row r="168" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="B168">
         <v>4</v>
@@ -25564,7 +25568,7 @@
     </row>
     <row r="169" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="B169">
         <v>6</v>
@@ -25704,7 +25708,7 @@
     </row>
     <row r="170" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="B170">
         <v>6</v>
@@ -25844,7 +25848,7 @@
     </row>
     <row r="171" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="B171">
         <v>6</v>
@@ -25984,7 +25988,7 @@
     </row>
     <row r="172" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="B172">
         <v>3</v>
@@ -26124,7 +26128,7 @@
     </row>
     <row r="173" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="B173">
         <v>1</v>
@@ -26264,7 +26268,7 @@
     </row>
     <row r="174" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="B174">
         <v>9</v>
@@ -26404,7 +26408,7 @@
     </row>
     <row r="175" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="B175">
         <v>3</v>
@@ -26544,7 +26548,7 @@
     </row>
     <row r="176" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="B176">
         <v>5</v>
@@ -26684,7 +26688,7 @@
     </row>
     <row r="177" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="B177">
         <v>6</v>
@@ -26824,7 +26828,7 @@
     </row>
     <row r="178" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="B178">
         <v>3</v>
@@ -26964,7 +26968,7 @@
     </row>
     <row r="179" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="B179">
         <v>10</v>
@@ -27104,7 +27108,7 @@
     </row>
     <row r="180" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="B180">
         <v>8</v>
@@ -27244,7 +27248,7 @@
     </row>
     <row r="181" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="B181">
         <v>4</v>
@@ -27384,7 +27388,7 @@
     </row>
     <row r="182" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="B182">
         <v>7</v>
@@ -27524,7 +27528,7 @@
     </row>
     <row r="183" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="B183">
         <v>2</v>
@@ -27664,7 +27668,7 @@
     </row>
     <row r="184" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="B184">
         <v>4</v>
@@ -27804,7 +27808,7 @@
     </row>
     <row r="185" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="B185">
         <v>6</v>
@@ -27944,7 +27948,7 @@
     </row>
     <row r="186" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="B186">
         <v>2</v>
@@ -28084,7 +28088,7 @@
     </row>
     <row r="187" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="B187">
         <v>2</v>
@@ -28224,7 +28228,7 @@
     </row>
     <row r="188" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="B188">
         <v>4</v>
@@ -28364,7 +28368,7 @@
     </row>
     <row r="189" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="B189">
         <v>3</v>
@@ -28504,7 +28508,7 @@
     </row>
     <row r="190" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="B190">
         <v>6</v>
@@ -28644,7 +28648,7 @@
     </row>
     <row r="191" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="B191">
         <v>5</v>
@@ -28784,7 +28788,7 @@
     </row>
     <row r="192" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="B192">
         <v>2</v>
@@ -28924,7 +28928,7 @@
     </row>
     <row r="193" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="B193">
         <v>5</v>
@@ -29064,7 +29068,7 @@
     </row>
     <row r="194" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="B194">
         <v>10</v>
@@ -29204,7 +29208,7 @@
     </row>
     <row r="195" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="B195">
         <v>2</v>
@@ -29344,7 +29348,7 @@
     </row>
     <row r="196" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="B196">
         <v>10</v>
@@ -29484,7 +29488,7 @@
     </row>
     <row r="197" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="B197">
         <v>4</v>
@@ -29624,7 +29628,7 @@
     </row>
     <row r="198" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="B198">
         <v>3</v>
@@ -29764,7 +29768,7 @@
     </row>
     <row r="199" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="B199">
         <v>4</v>
@@ -29904,7 +29908,7 @@
     </row>
     <row r="200" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="B200">
         <v>4</v>
@@ -30044,7 +30048,7 @@
     </row>
     <row r="201" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="B201">
         <v>7</v>
@@ -30184,7 +30188,7 @@
     </row>
     <row r="202" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="B202">
         <v>4</v>
@@ -30324,7 +30328,7 @@
     </row>
     <row r="203" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="B203">
         <v>1</v>
@@ -30464,7 +30468,7 @@
     </row>
     <row r="204" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="B204">
         <v>7</v>
@@ -30604,7 +30608,7 @@
     </row>
     <row r="205" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="B205">
         <v>1</v>
@@ -30744,7 +30748,7 @@
     </row>
     <row r="206" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="B206">
         <v>8</v>
@@ -30884,7 +30888,7 @@
     </row>
     <row r="207" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="B207">
         <v>8</v>
@@ -31024,7 +31028,7 @@
     </row>
     <row r="208" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="B208">
         <v>3</v>
@@ -31164,7 +31168,7 @@
     </row>
     <row r="209" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="B209">
         <v>5</v>
@@ -31304,7 +31308,7 @@
     </row>
     <row r="210" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="B210">
         <v>8</v>
@@ -31444,7 +31448,7 @@
     </row>
     <row r="211" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="B211">
         <v>9</v>
@@ -31584,7 +31588,7 @@
     </row>
     <row r="212" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="B212">
         <v>5</v>
@@ -31724,7 +31728,7 @@
     </row>
     <row r="213" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="B213">
         <v>7</v>
@@ -31864,7 +31868,7 @@
     </row>
     <row r="214" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="B214">
         <v>7</v>
@@ -32004,7 +32008,7 @@
     </row>
     <row r="215" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="B215">
         <v>6</v>
@@ -32144,7 +32148,7 @@
     </row>
     <row r="216" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="B216">
         <v>6</v>
@@ -32284,7 +32288,7 @@
     </row>
     <row r="217" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="B217">
         <v>6</v>
@@ -32424,7 +32428,7 @@
     </row>
     <row r="218" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="B218">
         <v>4</v>
@@ -32564,7 +32568,7 @@
     </row>
     <row r="219" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="B219">
         <v>10</v>
@@ -32704,7 +32708,7 @@
     </row>
     <row r="220" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="B220">
         <v>10</v>
@@ -32844,7 +32848,7 @@
     </row>
     <row r="221" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="B221">
         <v>8</v>
@@ -32984,7 +32988,7 @@
     </row>
     <row r="222" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="B222">
         <v>1</v>
@@ -33124,7 +33128,7 @@
     </row>
     <row r="223" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="B223">
         <v>8</v>
@@ -33264,7 +33268,7 @@
     </row>
     <row r="224" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="B224">
         <v>2</v>
@@ -33404,7 +33408,7 @@
     </row>
     <row r="225" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
       <c r="B225">
         <v>3</v>
@@ -33544,7 +33548,7 @@
     </row>
     <row r="226" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="B226">
         <v>5</v>
@@ -33684,7 +33688,7 @@
     </row>
     <row r="227" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="B227">
         <v>5</v>
@@ -33824,7 +33828,7 @@
     </row>
     <row r="228" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="B228">
         <v>8</v>
@@ -33964,7 +33968,7 @@
     </row>
     <row r="229" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="B229">
         <v>1</v>
@@ -34104,7 +34108,7 @@
     </row>
     <row r="230" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="B230">
         <v>3</v>
@@ -34244,7 +34248,7 @@
     </row>
     <row r="231" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="B231">
         <v>7</v>
@@ -34384,7 +34388,7 @@
     </row>
     <row r="232" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="B232">
         <v>10</v>
@@ -34524,7 +34528,7 @@
     </row>
     <row r="233" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
       <c r="B233">
         <v>6</v>
@@ -34664,7 +34668,7 @@
     </row>
     <row r="234" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="B234">
         <v>3</v>
@@ -34804,7 +34808,7 @@
     </row>
     <row r="235" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
       <c r="B235">
         <v>8</v>
@@ -34944,7 +34948,7 @@
     </row>
     <row r="236" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="B236">
         <v>8</v>
@@ -35084,7 +35088,7 @@
     </row>
     <row r="237" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="B237">
         <v>9</v>
@@ -35224,7 +35228,7 @@
     </row>
     <row r="238" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>282</v>
+        <v>264</v>
       </c>
       <c r="B238">
         <v>10</v>
@@ -35364,7 +35368,7 @@
     </row>
     <row r="239" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="B239">
         <v>1</v>
@@ -35504,7 +35508,7 @@
     </row>
     <row r="240" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
       <c r="B240">
         <v>2</v>
@@ -35644,7 +35648,7 @@
     </row>
     <row r="241" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
       <c r="B241">
         <v>1</v>
@@ -35784,7 +35788,7 @@
     </row>
     <row r="242" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
       <c r="B242">
         <v>4</v>
@@ -35924,7 +35928,7 @@
     </row>
     <row r="243" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>287</v>
+        <v>269</v>
       </c>
       <c r="B243">
         <v>8</v>
@@ -36064,7 +36068,7 @@
     </row>
     <row r="244" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>288</v>
+        <v>270</v>
       </c>
       <c r="B244">
         <v>8</v>
@@ -36204,7 +36208,7 @@
     </row>
     <row r="245" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>289</v>
+        <v>271</v>
       </c>
       <c r="B245">
         <v>9</v>
@@ -36344,7 +36348,7 @@
     </row>
     <row r="246" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="B246">
         <v>3</v>
@@ -36484,7 +36488,7 @@
     </row>
     <row r="247" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="B247">
         <v>3</v>
@@ -36624,7 +36628,7 @@
     </row>
     <row r="248" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="B248">
         <v>4</v>
@@ -36764,7 +36768,7 @@
     </row>
     <row r="249" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
       <c r="B249">
         <v>2</v>
@@ -36904,7 +36908,7 @@
     </row>
     <row r="250" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="B250">
         <v>9</v>
@@ -37044,7 +37048,7 @@
     </row>
     <row r="251" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
       <c r="B251">
         <v>7</v>
@@ -37184,7 +37188,7 @@
     </row>
     <row r="252" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>296</v>
+        <v>278</v>
       </c>
       <c r="B252">
         <v>2</v>
@@ -37324,7 +37328,7 @@
     </row>
     <row r="253" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="B253">
         <v>2</v>
@@ -37464,7 +37468,7 @@
     </row>
     <row r="254" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="B254">
         <v>4</v>
@@ -37604,7 +37608,7 @@
     </row>
     <row r="255" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="B255">
         <v>2</v>
@@ -37744,7 +37748,7 @@
     </row>
     <row r="256" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="B256">
         <v>5</v>
@@ -37884,7 +37888,7 @@
     </row>
     <row r="257" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
       <c r="B257">
         <v>2</v>
@@ -38024,7 +38028,7 @@
     </row>
     <row r="258" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>302</v>
+        <v>284</v>
       </c>
       <c r="B258">
         <v>3</v>
@@ -38164,7 +38168,7 @@
     </row>
     <row r="259" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>303</v>
+        <v>285</v>
       </c>
       <c r="B259">
         <v>8</v>
@@ -38304,7 +38308,7 @@
     </row>
     <row r="260" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>304</v>
+        <v>286</v>
       </c>
       <c r="B260">
         <v>5</v>
@@ -38444,7 +38448,7 @@
     </row>
     <row r="261" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>305</v>
+        <v>287</v>
       </c>
       <c r="B261">
         <v>1</v>
@@ -38584,7 +38588,7 @@
     </row>
     <row r="262" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>306</v>
+        <v>288</v>
       </c>
       <c r="B262">
         <v>6</v>
@@ -38724,7 +38728,7 @@
     </row>
     <row r="263" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>307</v>
+        <v>289</v>
       </c>
       <c r="B263">
         <v>4</v>
@@ -38864,7 +38868,7 @@
     </row>
     <row r="264" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>308</v>
+        <v>290</v>
       </c>
       <c r="B264">
         <v>5</v>
@@ -39004,7 +39008,7 @@
     </row>
     <row r="265" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>309</v>
+        <v>291</v>
       </c>
       <c r="B265">
         <v>10</v>
@@ -39144,7 +39148,7 @@
     </row>
     <row r="266" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
       <c r="B266">
         <v>5</v>
@@ -39284,7 +39288,7 @@
     </row>
     <row r="267" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
-        <v>311</v>
+        <v>293</v>
       </c>
       <c r="B267">
         <v>3</v>
@@ -39424,7 +39428,7 @@
     </row>
     <row r="268" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>312</v>
+        <v>294</v>
       </c>
       <c r="B268">
         <v>5</v>
@@ -39564,7 +39568,7 @@
     </row>
     <row r="269" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>313</v>
+        <v>295</v>
       </c>
       <c r="B269">
         <v>3</v>
@@ -39704,7 +39708,7 @@
     </row>
     <row r="270" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="B270">
         <v>3</v>
@@ -39844,7 +39848,7 @@
     </row>
     <row r="271" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="B271">
         <v>4</v>
@@ -39984,7 +39988,7 @@
     </row>
     <row r="272" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="B272">
         <v>2</v>
@@ -40124,7 +40128,7 @@
     </row>
     <row r="273" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="B273">
         <v>2</v>
@@ -40264,7 +40268,7 @@
     </row>
     <row r="274" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="B274">
         <v>3</v>
@@ -40404,7 +40408,7 @@
     </row>
     <row r="275" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="B275">
         <v>9</v>
@@ -40544,7 +40548,7 @@
     </row>
     <row r="276" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="B276">
         <v>7</v>
@@ -40684,7 +40688,7 @@
     </row>
     <row r="277" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="B277">
         <v>1</v>
@@ -40824,7 +40828,7 @@
     </row>
     <row r="278" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="B278">
         <v>9</v>
@@ -40964,7 +40968,7 @@
     </row>
     <row r="279" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="B279">
         <v>8</v>
@@ -41104,7 +41108,7 @@
     </row>
     <row r="280" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
-        <v>324</v>
+        <v>306</v>
       </c>
       <c r="B280">
         <v>8</v>
@@ -41244,7 +41248,7 @@
     </row>
     <row r="281" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
-        <v>325</v>
+        <v>307</v>
       </c>
       <c r="B281">
         <v>3</v>
@@ -41384,7 +41388,7 @@
     </row>
     <row r="282" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
       <c r="B282">
         <v>10</v>
@@ -41524,7 +41528,7 @@
     </row>
     <row r="283" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
-        <v>327</v>
+        <v>309</v>
       </c>
       <c r="B283">
         <v>4</v>
@@ -41664,7 +41668,7 @@
     </row>
     <row r="284" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
-        <v>328</v>
+        <v>310</v>
       </c>
       <c r="B284">
         <v>7</v>
@@ -41804,7 +41808,7 @@
     </row>
     <row r="285" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="B285">
         <v>1</v>
@@ -41944,7 +41948,7 @@
     </row>
     <row r="286" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
-        <v>330</v>
+        <v>312</v>
       </c>
       <c r="B286">
         <v>1</v>
@@ -42084,7 +42088,7 @@
     </row>
     <row r="287" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>331</v>
+        <v>313</v>
       </c>
       <c r="B287">
         <v>10</v>
@@ -42224,7 +42228,7 @@
     </row>
     <row r="288" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
-        <v>332</v>
+        <v>314</v>
       </c>
       <c r="B288">
         <v>2</v>
@@ -42364,7 +42368,7 @@
     </row>
     <row r="289" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="B289">
         <v>1</v>
@@ -42504,7 +42508,7 @@
     </row>
     <row r="290" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
-        <v>334</v>
+        <v>316</v>
       </c>
       <c r="B290">
         <v>2</v>
@@ -42644,7 +42648,7 @@
     </row>
     <row r="291" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
-        <v>335</v>
+        <v>317</v>
       </c>
       <c r="B291">
         <v>5</v>
@@ -42784,7 +42788,7 @@
     </row>
     <row r="292" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
-        <v>336</v>
+        <v>318</v>
       </c>
       <c r="B292">
         <v>4</v>
@@ -42924,7 +42928,7 @@
     </row>
     <row r="293" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
-        <v>337</v>
+        <v>319</v>
       </c>
       <c r="B293">
         <v>10</v>
@@ -43064,7 +43068,7 @@
     </row>
     <row r="294" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
-        <v>338</v>
+        <v>320</v>
       </c>
       <c r="B294">
         <v>6</v>
@@ -43204,7 +43208,7 @@
     </row>
     <row r="295" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
-        <v>339</v>
+        <v>321</v>
       </c>
       <c r="B295">
         <v>6</v>
@@ -43344,7 +43348,7 @@
     </row>
     <row r="296" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
-        <v>340</v>
+        <v>322</v>
       </c>
       <c r="B296">
         <v>6</v>
@@ -43484,7 +43488,7 @@
     </row>
     <row r="297" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
-        <v>341</v>
+        <v>323</v>
       </c>
       <c r="B297">
         <v>5</v>
@@ -43624,7 +43628,7 @@
     </row>
     <row r="298" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
-        <v>342</v>
+        <v>324</v>
       </c>
       <c r="B298">
         <v>5</v>
@@ -43764,7 +43768,7 @@
     </row>
     <row r="299" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
-        <v>343</v>
+        <v>325</v>
       </c>
       <c r="B299">
         <v>6</v>
@@ -43904,7 +43908,7 @@
     </row>
     <row r="300" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
-        <v>344</v>
+        <v>326</v>
       </c>
       <c r="B300">
         <v>1</v>
@@ -44044,7 +44048,7 @@
     </row>
     <row r="301" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
-        <v>345</v>
+        <v>327</v>
       </c>
       <c r="B301">
         <v>8</v>
@@ -44184,7 +44188,7 @@
     </row>
     <row r="302" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
-        <v>346</v>
+        <v>328</v>
       </c>
       <c r="B302">
         <v>3</v>
@@ -44324,7 +44328,7 @@
     </row>
     <row r="303" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
-        <v>347</v>
+        <v>329</v>
       </c>
       <c r="B303">
         <v>7</v>
@@ -44464,7 +44468,7 @@
     </row>
     <row r="304" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
-        <v>348</v>
+        <v>330</v>
       </c>
       <c r="B304">
         <v>9</v>
@@ -44604,7 +44608,7 @@
     </row>
     <row r="305" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
-        <v>349</v>
+        <v>331</v>
       </c>
       <c r="B305">
         <v>1</v>
@@ -44744,7 +44748,7 @@
     </row>
     <row r="306" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
-        <v>350</v>
+        <v>332</v>
       </c>
       <c r="B306">
         <v>3</v>
@@ -44884,7 +44888,7 @@
     </row>
     <row r="307" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
-        <v>351</v>
+        <v>333</v>
       </c>
       <c r="B307">
         <v>6</v>
@@ -45024,7 +45028,7 @@
     </row>
     <row r="308" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
       <c r="B308">
         <v>10</v>
@@ -45164,7 +45168,7 @@
     </row>
     <row r="309" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
-        <v>353</v>
+        <v>335</v>
       </c>
       <c r="B309">
         <v>6</v>
@@ -45304,7 +45308,7 @@
     </row>
     <row r="310" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
-        <v>354</v>
+        <v>336</v>
       </c>
       <c r="B310">
         <v>9</v>
@@ -45444,7 +45448,7 @@
     </row>
     <row r="311" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
-        <v>355</v>
+        <v>337</v>
       </c>
       <c r="B311">
         <v>9</v>
@@ -45584,7 +45588,7 @@
     </row>
     <row r="312" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
-        <v>356</v>
+        <v>338</v>
       </c>
       <c r="B312">
         <v>3</v>
@@ -45724,7 +45728,7 @@
     </row>
     <row r="313" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
-        <v>357</v>
+        <v>339</v>
       </c>
       <c r="B313">
         <v>10</v>
@@ -45864,7 +45868,7 @@
     </row>
     <row r="314" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
-        <v>358</v>
+        <v>340</v>
       </c>
       <c r="B314">
         <v>5</v>
@@ -46004,7 +46008,7 @@
     </row>
     <row r="315" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
-        <v>359</v>
+        <v>341</v>
       </c>
       <c r="B315">
         <v>2</v>
@@ -46144,7 +46148,7 @@
     </row>
     <row r="316" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="B316">
         <v>4</v>
@@ -46284,7 +46288,7 @@
     </row>
     <row r="317" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
-        <v>361</v>
+        <v>343</v>
       </c>
       <c r="B317">
         <v>6</v>
@@ -46424,7 +46428,7 @@
     </row>
     <row r="318" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
-        <v>362</v>
+        <v>344</v>
       </c>
       <c r="B318">
         <v>1</v>
@@ -46564,7 +46568,7 @@
     </row>
     <row r="319" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
-        <v>363</v>
+        <v>345</v>
       </c>
       <c r="B319">
         <v>2</v>
@@ -46704,7 +46708,7 @@
     </row>
     <row r="320" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
-        <v>364</v>
+        <v>346</v>
       </c>
       <c r="B320">
         <v>2</v>
@@ -46844,7 +46848,7 @@
     </row>
     <row r="321" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
-        <v>365</v>
+        <v>347</v>
       </c>
       <c r="B321">
         <v>5</v>
@@ -46984,7 +46988,7 @@
     </row>
     <row r="322" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
-        <v>366</v>
+        <v>348</v>
       </c>
       <c r="B322">
         <v>7</v>
@@ -47124,7 +47128,7 @@
     </row>
     <row r="323" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
-        <v>367</v>
+        <v>349</v>
       </c>
       <c r="B323">
         <v>3</v>
@@ -47264,7 +47268,7 @@
     </row>
     <row r="324" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
-        <v>368</v>
+        <v>350</v>
       </c>
       <c r="B324">
         <v>3</v>
@@ -47404,7 +47408,7 @@
     </row>
     <row r="325" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
-        <v>369</v>
+        <v>351</v>
       </c>
       <c r="B325">
         <v>5</v>
@@ -47544,7 +47548,7 @@
     </row>
     <row r="326" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
-        <v>370</v>
+        <v>352</v>
       </c>
       <c r="B326">
         <v>8</v>
@@ -47684,7 +47688,7 @@
     </row>
     <row r="327" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
-        <v>371</v>
+        <v>353</v>
       </c>
       <c r="B327">
         <v>10</v>
@@ -47824,7 +47828,7 @@
     </row>
     <row r="328" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
-        <v>372</v>
+        <v>354</v>
       </c>
       <c r="B328">
         <v>10</v>
@@ -47964,7 +47968,7 @@
     </row>
     <row r="329" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
       <c r="B329">
         <v>10</v>
@@ -48104,7 +48108,7 @@
     </row>
     <row r="330" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
-        <v>374</v>
+        <v>356</v>
       </c>
       <c r="B330">
         <v>3</v>
@@ -48244,7 +48248,7 @@
     </row>
     <row r="331" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
-        <v>375</v>
+        <v>357</v>
       </c>
       <c r="B331">
         <v>2</v>
@@ -48384,7 +48388,7 @@
     </row>
     <row r="332" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
-        <v>376</v>
+        <v>358</v>
       </c>
       <c r="B332">
         <v>1</v>
@@ -48524,7 +48528,7 @@
     </row>
     <row r="333" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
-        <v>377</v>
+        <v>359</v>
       </c>
       <c r="B333">
         <v>1</v>
@@ -48664,7 +48668,7 @@
     </row>
     <row r="334" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
-        <v>378</v>
+        <v>360</v>
       </c>
       <c r="B334">
         <v>3</v>
@@ -48804,7 +48808,7 @@
     </row>
     <row r="335" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
-        <v>379</v>
+        <v>361</v>
       </c>
       <c r="B335">
         <v>6</v>
@@ -48944,7 +48948,7 @@
     </row>
     <row r="336" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
-        <v>380</v>
+        <v>362</v>
       </c>
       <c r="B336">
         <v>8</v>
@@ -49084,7 +49088,7 @@
     </row>
     <row r="337" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
-        <v>381</v>
+        <v>363</v>
       </c>
       <c r="B337">
         <v>6</v>
@@ -49224,7 +49228,7 @@
     </row>
     <row r="338" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
       <c r="B338">
         <v>8</v>
@@ -49364,7 +49368,7 @@
     </row>
     <row r="339" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
-        <v>383</v>
+        <v>365</v>
       </c>
       <c r="B339">
         <v>5</v>
@@ -49504,7 +49508,7 @@
     </row>
     <row r="340" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
-        <v>384</v>
+        <v>366</v>
       </c>
       <c r="B340">
         <v>1</v>
@@ -49644,7 +49648,7 @@
     </row>
     <row r="341" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
-        <v>385</v>
+        <v>367</v>
       </c>
       <c r="B341">
         <v>1</v>
@@ -49784,7 +49788,7 @@
     </row>
     <row r="342" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
-        <v>386</v>
+        <v>368</v>
       </c>
       <c r="B342">
         <v>1</v>
@@ -49924,7 +49928,7 @@
     </row>
     <row r="343" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
-        <v>387</v>
+        <v>369</v>
       </c>
       <c r="B343">
         <v>3</v>
@@ -50064,7 +50068,7 @@
     </row>
     <row r="344" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
-        <v>388</v>
+        <v>370</v>
       </c>
       <c r="B344">
         <v>4</v>
@@ -50204,7 +50208,7 @@
     </row>
     <row r="345" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
-        <v>389</v>
+        <v>371</v>
       </c>
       <c r="B345">
         <v>2</v>
@@ -50344,7 +50348,7 @@
     </row>
     <row r="346" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
-        <v>390</v>
+        <v>372</v>
       </c>
       <c r="B346">
         <v>5</v>
@@ -50484,7 +50488,7 @@
     </row>
     <row r="347" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
-        <v>391</v>
+        <v>373</v>
       </c>
       <c r="B347">
         <v>6</v>
@@ -50624,7 +50628,7 @@
     </row>
     <row r="348" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
-        <v>392</v>
+        <v>374</v>
       </c>
       <c r="B348">
         <v>9</v>
@@ -50764,7 +50768,7 @@
     </row>
     <row r="349" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
-        <v>393</v>
+        <v>375</v>
       </c>
       <c r="B349">
         <v>3</v>
@@ -50904,7 +50908,7 @@
     </row>
     <row r="350" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
-        <v>394</v>
+        <v>376</v>
       </c>
       <c r="B350">
         <v>7</v>
@@ -51044,7 +51048,7 @@
     </row>
     <row r="351" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
-        <v>395</v>
+        <v>377</v>
       </c>
       <c r="B351">
         <v>8</v>
@@ -51184,7 +51188,7 @@
     </row>
     <row r="352" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
-        <v>396</v>
+        <v>378</v>
       </c>
       <c r="B352">
         <v>9</v>
@@ -51324,7 +51328,7 @@
     </row>
     <row r="353" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
-        <v>397</v>
+        <v>379</v>
       </c>
       <c r="B353">
         <v>3</v>
@@ -51464,7 +51468,7 @@
     </row>
     <row r="354" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
-        <v>398</v>
+        <v>380</v>
       </c>
       <c r="B354">
         <v>7</v>
@@ -51604,7 +51608,7 @@
     </row>
     <row r="355" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
       <c r="B355">
         <v>1</v>
@@ -51744,7 +51748,7 @@
     </row>
     <row r="356" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="B356">
         <v>6</v>
@@ -51884,7 +51888,7 @@
     </row>
     <row r="357" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
-        <v>401</v>
+        <v>383</v>
       </c>
       <c r="B357">
         <v>8</v>
@@ -52024,7 +52028,7 @@
     </row>
     <row r="358" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
-        <v>402</v>
+        <v>384</v>
       </c>
       <c r="B358">
         <v>2</v>
@@ -52164,7 +52168,7 @@
     </row>
     <row r="359" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
-        <v>403</v>
+        <v>385</v>
       </c>
       <c r="B359">
         <v>6</v>
@@ -52304,7 +52308,7 @@
     </row>
     <row r="360" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="B360">
         <v>1</v>
@@ -52444,7 +52448,7 @@
     </row>
     <row r="361" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
       <c r="B361">
         <v>9</v>
@@ -52584,7 +52588,7 @@
     </row>
     <row r="362" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
-        <v>406</v>
+        <v>388</v>
       </c>
       <c r="B362">
         <v>10</v>
@@ -52724,7 +52728,7 @@
     </row>
     <row r="363" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
       <c r="B363">
         <v>6</v>
@@ -52864,7 +52868,7 @@
     </row>
     <row r="364" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
       <c r="B364">
         <v>1</v>
@@ -53004,7 +53008,7 @@
     </row>
     <row r="365" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
-        <v>409</v>
+        <v>391</v>
       </c>
       <c r="B365">
         <v>10</v>
@@ -53144,7 +53148,7 @@
     </row>
     <row r="366" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
-        <v>410</v>
+        <v>392</v>
       </c>
       <c r="B366">
         <v>7</v>
@@ -53284,7 +53288,7 @@
     </row>
     <row r="367" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
       <c r="B367">
         <v>4</v>
@@ -53424,7 +53428,7 @@
     </row>
     <row r="368" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="B368">
         <v>7</v>
@@ -53564,7 +53568,7 @@
     </row>
     <row r="369" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
-        <v>413</v>
+        <v>395</v>
       </c>
       <c r="B369">
         <v>8</v>
@@ -53704,7 +53708,7 @@
     </row>
     <row r="370" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
-        <v>414</v>
+        <v>396</v>
       </c>
       <c r="B370">
         <v>10</v>
@@ -53844,7 +53848,7 @@
     </row>
     <row r="371" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
-        <v>415</v>
+        <v>397</v>
       </c>
       <c r="B371">
         <v>9</v>
@@ -53984,7 +53988,7 @@
     </row>
     <row r="372" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="B372">
         <v>3</v>
@@ -54124,7 +54128,7 @@
     </row>
     <row r="373" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
-        <v>417</v>
+        <v>399</v>
       </c>
       <c r="B373">
         <v>6</v>
@@ -54264,7 +54268,7 @@
     </row>
     <row r="374" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
-        <v>418</v>
+        <v>400</v>
       </c>
       <c r="B374">
         <v>10</v>
@@ -54404,7 +54408,7 @@
     </row>
     <row r="375" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
-        <v>419</v>
+        <v>401</v>
       </c>
       <c r="B375">
         <v>10</v>
@@ -54544,7 +54548,7 @@
     </row>
     <row r="376" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
-        <v>420</v>
+        <v>402</v>
       </c>
       <c r="B376">
         <v>7</v>
@@ -54684,7 +54688,7 @@
     </row>
     <row r="377" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
-        <v>421</v>
+        <v>403</v>
       </c>
       <c r="B377">
         <v>6</v>
@@ -54824,7 +54828,7 @@
     </row>
     <row r="378" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
-        <v>422</v>
+        <v>404</v>
       </c>
       <c r="B378">
         <v>9</v>
@@ -54964,7 +54968,7 @@
     </row>
     <row r="379" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
-        <v>423</v>
+        <v>405</v>
       </c>
       <c r="B379">
         <v>3</v>
@@ -55104,7 +55108,7 @@
     </row>
     <row r="380" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
-        <v>424</v>
+        <v>406</v>
       </c>
       <c r="B380">
         <v>6</v>
@@ -55244,7 +55248,7 @@
     </row>
     <row r="381" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
-        <v>425</v>
+        <v>407</v>
       </c>
       <c r="B381">
         <v>2</v>
@@ -55384,7 +55388,7 @@
     </row>
     <row r="382" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
-        <v>426</v>
+        <v>408</v>
       </c>
       <c r="B382">
         <v>2</v>
@@ -55524,7 +55528,7 @@
     </row>
     <row r="383" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
-        <v>427</v>
+        <v>409</v>
       </c>
       <c r="B383">
         <v>10</v>
@@ -55664,7 +55668,7 @@
     </row>
     <row r="384" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
-        <v>428</v>
+        <v>410</v>
       </c>
       <c r="B384">
         <v>10</v>
@@ -55804,7 +55808,7 @@
     </row>
     <row r="385" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A385" t="s">
-        <v>429</v>
+        <v>411</v>
       </c>
       <c r="B385">
         <v>8</v>
@@ -55944,7 +55948,7 @@
     </row>
     <row r="386" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A386" t="s">
-        <v>430</v>
+        <v>412</v>
       </c>
       <c r="B386">
         <v>7</v>
@@ -56084,7 +56088,7 @@
     </row>
     <row r="387" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A387" t="s">
-        <v>431</v>
+        <v>413</v>
       </c>
       <c r="B387">
         <v>6</v>
@@ -56224,7 +56228,7 @@
     </row>
     <row r="388" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A388" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
       <c r="B388">
         <v>5</v>
@@ -56364,7 +56368,7 @@
     </row>
     <row r="389" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A389" t="s">
-        <v>433</v>
+        <v>415</v>
       </c>
       <c r="B389">
         <v>1</v>
@@ -56504,7 +56508,7 @@
     </row>
     <row r="390" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A390" t="s">
-        <v>434</v>
+        <v>416</v>
       </c>
       <c r="B390">
         <v>5</v>
@@ -56644,7 +56648,7 @@
     </row>
     <row r="391" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A391" t="s">
-        <v>435</v>
+        <v>417</v>
       </c>
       <c r="B391">
         <v>4</v>
@@ -56784,7 +56788,7 @@
     </row>
     <row r="392" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
-        <v>436</v>
+        <v>418</v>
       </c>
       <c r="B392">
         <v>9</v>
@@ -56924,7 +56928,7 @@
     </row>
     <row r="393" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A393" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
       <c r="B393">
         <v>10</v>
@@ -57064,7 +57068,7 @@
     </row>
     <row r="394" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A394" t="s">
-        <v>438</v>
+        <v>420</v>
       </c>
       <c r="B394">
         <v>7</v>
@@ -57204,7 +57208,7 @@
     </row>
     <row r="395" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A395" t="s">
-        <v>439</v>
+        <v>421</v>
       </c>
       <c r="B395">
         <v>7</v>
@@ -57344,7 +57348,7 @@
     </row>
     <row r="396" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A396" t="s">
-        <v>440</v>
+        <v>422</v>
       </c>
       <c r="B396">
         <v>2</v>
@@ -57484,7 +57488,7 @@
     </row>
     <row r="397" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
-        <v>441</v>
+        <v>423</v>
       </c>
       <c r="B397">
         <v>5</v>
@@ -57624,7 +57628,7 @@
     </row>
     <row r="398" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
-        <v>442</v>
+        <v>424</v>
       </c>
       <c r="B398">
         <v>5</v>
@@ -57764,7 +57768,7 @@
     </row>
     <row r="399" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
-        <v>443</v>
+        <v>425</v>
       </c>
       <c r="B399">
         <v>1</v>
@@ -57904,7 +57908,7 @@
     </row>
     <row r="400" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
-        <v>444</v>
+        <v>426</v>
       </c>
       <c r="B400">
         <v>8</v>
@@ -58044,7 +58048,7 @@
     </row>
     <row r="401" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
-        <v>445</v>
+        <v>427</v>
       </c>
       <c r="B401">
         <v>8</v>
@@ -58184,7 +58188,7 @@
     </row>
     <row r="402" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
-        <v>446</v>
+        <v>428</v>
       </c>
       <c r="B402">
         <v>1</v>
@@ -58324,7 +58328,7 @@
     </row>
     <row r="403" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
-        <v>447</v>
+        <v>429</v>
       </c>
       <c r="B403">
         <v>10</v>
@@ -58464,7 +58468,7 @@
     </row>
     <row r="404" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
-        <v>448</v>
+        <v>430</v>
       </c>
       <c r="B404">
         <v>7</v>
@@ -58604,7 +58608,7 @@
     </row>
     <row r="405" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
-        <v>449</v>
+        <v>431</v>
       </c>
       <c r="B405">
         <v>7</v>
@@ -58744,7 +58748,7 @@
     </row>
     <row r="406" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
-        <v>450</v>
+        <v>432</v>
       </c>
       <c r="B406">
         <v>2</v>
@@ -58884,7 +58888,7 @@
     </row>
     <row r="407" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
-        <v>451</v>
+        <v>433</v>
       </c>
       <c r="B407">
         <v>1</v>
@@ -59024,7 +59028,7 @@
     </row>
     <row r="408" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
-        <v>452</v>
+        <v>434</v>
       </c>
       <c r="B408">
         <v>6</v>
@@ -59164,7 +59168,7 @@
     </row>
     <row r="409" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
-        <v>453</v>
+        <v>435</v>
       </c>
       <c r="B409">
         <v>1</v>
@@ -59304,7 +59308,7 @@
     </row>
     <row r="410" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
-        <v>454</v>
+        <v>436</v>
       </c>
       <c r="B410">
         <v>9</v>
@@ -59444,7 +59448,7 @@
     </row>
     <row r="411" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
       <c r="B411">
         <v>10</v>
@@ -59584,7 +59588,7 @@
     </row>
     <row r="412" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
-        <v>456</v>
+        <v>438</v>
       </c>
       <c r="B412">
         <v>8</v>
@@ -59724,7 +59728,7 @@
     </row>
     <row r="413" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
-        <v>457</v>
+        <v>439</v>
       </c>
       <c r="B413">
         <v>3</v>
@@ -59864,7 +59868,7 @@
     </row>
     <row r="414" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
-        <v>458</v>
+        <v>440</v>
       </c>
       <c r="B414">
         <v>4</v>
@@ -60004,7 +60008,7 @@
     </row>
     <row r="415" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
-        <v>459</v>
+        <v>441</v>
       </c>
       <c r="B415">
         <v>3</v>
@@ -60144,7 +60148,7 @@
     </row>
     <row r="416" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A416" t="s">
-        <v>460</v>
+        <v>442</v>
       </c>
       <c r="B416">
         <v>2</v>
@@ -60284,7 +60288,7 @@
     </row>
     <row r="417" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
-        <v>461</v>
+        <v>443</v>
       </c>
       <c r="B417">
         <v>9</v>
@@ -60424,7 +60428,7 @@
     </row>
     <row r="418" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A418" t="s">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c r="B418">
         <v>4</v>
@@ -60564,7 +60568,7 @@
     </row>
     <row r="419" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A419" t="s">
-        <v>463</v>
+        <v>445</v>
       </c>
       <c r="B419">
         <v>1</v>
@@ -60704,7 +60708,7 @@
     </row>
     <row r="420" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A420" t="s">
-        <v>464</v>
+        <v>446</v>
       </c>
       <c r="B420">
         <v>7</v>
@@ -60844,7 +60848,7 @@
     </row>
     <row r="421" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A421" t="s">
-        <v>465</v>
+        <v>447</v>
       </c>
       <c r="B421">
         <v>2</v>
@@ -60984,7 +60988,7 @@
     </row>
     <row r="422" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A422" t="s">
-        <v>466</v>
+        <v>448</v>
       </c>
       <c r="B422">
         <v>6</v>
@@ -61124,7 +61128,7 @@
     </row>
     <row r="423" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A423" t="s">
-        <v>467</v>
+        <v>449</v>
       </c>
       <c r="B423">
         <v>9</v>
@@ -61264,7 +61268,7 @@
     </row>
     <row r="424" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A424" t="s">
-        <v>468</v>
+        <v>450</v>
       </c>
       <c r="B424">
         <v>9</v>
@@ -61404,7 +61408,7 @@
     </row>
     <row r="425" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A425" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
       <c r="B425">
         <v>7</v>
@@ -61544,7 +61548,7 @@
     </row>
     <row r="426" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A426" t="s">
-        <v>470</v>
+        <v>452</v>
       </c>
       <c r="B426">
         <v>5</v>
@@ -61684,7 +61688,7 @@
     </row>
     <row r="427" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A427" t="s">
-        <v>471</v>
+        <v>453</v>
       </c>
       <c r="B427">
         <v>9</v>
@@ -61824,7 +61828,7 @@
     </row>
     <row r="428" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A428" t="s">
-        <v>472</v>
+        <v>454</v>
       </c>
       <c r="B428">
         <v>1</v>
@@ -61964,7 +61968,7 @@
     </row>
     <row r="429" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A429" t="s">
-        <v>473</v>
+        <v>455</v>
       </c>
       <c r="B429">
         <v>2</v>
@@ -62104,7 +62108,7 @@
     </row>
     <row r="430" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A430" t="s">
-        <v>474</v>
+        <v>456</v>
       </c>
       <c r="B430">
         <v>7</v>
@@ -62244,7 +62248,7 @@
     </row>
     <row r="431" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A431" t="s">
-        <v>475</v>
+        <v>457</v>
       </c>
       <c r="B431">
         <v>8</v>
@@ -62384,7 +62388,7 @@
     </row>
     <row r="432" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A432" t="s">
-        <v>476</v>
+        <v>458</v>
       </c>
       <c r="B432">
         <v>8</v>
@@ -62524,7 +62528,7 @@
     </row>
     <row r="433" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A433" t="s">
-        <v>477</v>
+        <v>459</v>
       </c>
       <c r="B433">
         <v>9</v>
@@ -62664,7 +62668,7 @@
     </row>
     <row r="434" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A434" t="s">
-        <v>478</v>
+        <v>460</v>
       </c>
       <c r="B434">
         <v>6</v>
@@ -62804,7 +62808,7 @@
     </row>
     <row r="435" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A435" t="s">
-        <v>479</v>
+        <v>461</v>
       </c>
       <c r="B435">
         <v>4</v>
@@ -62944,7 +62948,7 @@
     </row>
     <row r="436" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A436" t="s">
-        <v>480</v>
+        <v>462</v>
       </c>
       <c r="B436">
         <v>7</v>
@@ -63084,7 +63088,7 @@
     </row>
     <row r="437" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A437" t="s">
-        <v>481</v>
+        <v>463</v>
       </c>
       <c r="B437">
         <v>10</v>
@@ -63224,7 +63228,7 @@
     </row>
     <row r="438" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A438" t="s">
-        <v>482</v>
+        <v>464</v>
       </c>
       <c r="B438">
         <v>3</v>
@@ -63364,7 +63368,7 @@
     </row>
     <row r="439" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A439" t="s">
-        <v>483</v>
+        <v>465</v>
       </c>
       <c r="B439">
         <v>2</v>
@@ -63504,7 +63508,7 @@
     </row>
     <row r="440" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A440" t="s">
-        <v>484</v>
+        <v>466</v>
       </c>
       <c r="B440">
         <v>8</v>
@@ -63644,7 +63648,7 @@
     </row>
     <row r="441" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A441" t="s">
-        <v>485</v>
+        <v>467</v>
       </c>
       <c r="B441">
         <v>6</v>
@@ -63784,7 +63788,7 @@
     </row>
     <row r="442" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A442" t="s">
-        <v>486</v>
+        <v>468</v>
       </c>
       <c r="B442">
         <v>3</v>
@@ -63924,7 +63928,7 @@
     </row>
     <row r="443" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A443" t="s">
-        <v>487</v>
+        <v>469</v>
       </c>
       <c r="B443">
         <v>5</v>
@@ -64064,7 +64068,7 @@
     </row>
     <row r="444" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A444" t="s">
-        <v>488</v>
+        <v>470</v>
       </c>
       <c r="B444">
         <v>2</v>
@@ -64204,7 +64208,7 @@
     </row>
     <row r="445" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A445" t="s">
-        <v>489</v>
+        <v>471</v>
       </c>
       <c r="B445">
         <v>7</v>
@@ -64344,7 +64348,7 @@
     </row>
     <row r="446" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A446" t="s">
-        <v>490</v>
+        <v>472</v>
       </c>
       <c r="B446">
         <v>2</v>
@@ -64484,7 +64488,7 @@
     </row>
     <row r="447" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A447" t="s">
-        <v>491</v>
+        <v>473</v>
       </c>
       <c r="B447">
         <v>5</v>
@@ -64624,7 +64628,7 @@
     </row>
     <row r="448" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A448" t="s">
-        <v>492</v>
+        <v>474</v>
       </c>
       <c r="B448">
         <v>10</v>
@@ -64764,7 +64768,7 @@
     </row>
     <row r="449" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A449" t="s">
-        <v>493</v>
+        <v>475</v>
       </c>
       <c r="B449">
         <v>7</v>
@@ -64904,7 +64908,7 @@
     </row>
     <row r="450" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A450" t="s">
-        <v>494</v>
+        <v>476</v>
       </c>
       <c r="B450">
         <v>6</v>
@@ -65044,7 +65048,7 @@
     </row>
     <row r="451" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A451" t="s">
-        <v>495</v>
+        <v>477</v>
       </c>
       <c r="B451">
         <v>3</v>
@@ -65184,7 +65188,7 @@
     </row>
     <row r="452" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A452" t="s">
-        <v>496</v>
+        <v>478</v>
       </c>
       <c r="B452">
         <v>5</v>
@@ -65324,7 +65328,7 @@
     </row>
     <row r="453" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A453" t="s">
-        <v>497</v>
+        <v>479</v>
       </c>
       <c r="B453">
         <v>6</v>
@@ -65464,7 +65468,7 @@
     </row>
     <row r="454" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A454" t="s">
-        <v>498</v>
+        <v>480</v>
       </c>
       <c r="B454">
         <v>1</v>
@@ -65604,7 +65608,7 @@
     </row>
     <row r="455" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A455" t="s">
-        <v>499</v>
+        <v>481</v>
       </c>
       <c r="B455">
         <v>2</v>
@@ -65744,7 +65748,7 @@
     </row>
     <row r="456" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A456" t="s">
-        <v>500</v>
+        <v>482</v>
       </c>
       <c r="B456">
         <v>10</v>
@@ -65884,7 +65888,7 @@
     </row>
     <row r="457" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A457" t="s">
-        <v>501</v>
+        <v>483</v>
       </c>
       <c r="B457">
         <v>7</v>
@@ -66024,7 +66028,7 @@
     </row>
     <row r="458" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A458" t="s">
-        <v>502</v>
+        <v>484</v>
       </c>
       <c r="B458">
         <v>1</v>
@@ -66164,7 +66168,7 @@
     </row>
     <row r="459" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A459" t="s">
-        <v>503</v>
+        <v>485</v>
       </c>
       <c r="B459">
         <v>10</v>
@@ -66304,7 +66308,7 @@
     </row>
     <row r="460" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A460" t="s">
-        <v>504</v>
+        <v>486</v>
       </c>
       <c r="B460">
         <v>9</v>
@@ -66444,7 +66448,7 @@
     </row>
     <row r="461" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A461" t="s">
-        <v>505</v>
+        <v>487</v>
       </c>
       <c r="B461">
         <v>7</v>
@@ -66584,7 +66588,7 @@
     </row>
     <row r="462" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A462" t="s">
-        <v>506</v>
+        <v>488</v>
       </c>
       <c r="B462">
         <v>1</v>
@@ -66724,7 +66728,7 @@
     </row>
     <row r="463" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A463" t="s">
-        <v>507</v>
+        <v>489</v>
       </c>
       <c r="B463">
         <v>3</v>
@@ -66864,7 +66868,7 @@
     </row>
     <row r="464" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A464" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="B464">
         <v>2</v>
@@ -67004,7 +67008,7 @@
     </row>
     <row r="465" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A465" t="s">
-        <v>509</v>
+        <v>491</v>
       </c>
       <c r="B465">
         <v>7</v>
@@ -67144,7 +67148,7 @@
     </row>
     <row r="466" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A466" t="s">
-        <v>510</v>
+        <v>492</v>
       </c>
       <c r="B466">
         <v>7</v>
@@ -67284,7 +67288,7 @@
     </row>
     <row r="467" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A467" t="s">
-        <v>511</v>
+        <v>493</v>
       </c>
       <c r="B467">
         <v>1</v>
@@ -67424,7 +67428,7 @@
     </row>
     <row r="468" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A468" t="s">
-        <v>512</v>
+        <v>494</v>
       </c>
       <c r="B468">
         <v>1</v>
@@ -67564,7 +67568,7 @@
     </row>
     <row r="469" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A469" t="s">
-        <v>513</v>
+        <v>495</v>
       </c>
       <c r="B469">
         <v>5</v>
@@ -67704,7 +67708,7 @@
     </row>
     <row r="470" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A470" t="s">
-        <v>514</v>
+        <v>496</v>
       </c>
       <c r="B470">
         <v>3</v>
@@ -67844,7 +67848,7 @@
     </row>
     <row r="471" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A471" t="s">
-        <v>515</v>
+        <v>497</v>
       </c>
       <c r="B471">
         <v>2</v>
@@ -67984,7 +67988,7 @@
     </row>
     <row r="472" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A472" t="s">
-        <v>516</v>
+        <v>498</v>
       </c>
       <c r="B472">
         <v>7</v>
@@ -68124,7 +68128,7 @@
     </row>
     <row r="473" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A473" t="s">
-        <v>517</v>
+        <v>499</v>
       </c>
       <c r="B473">
         <v>4</v>
@@ -68264,7 +68268,7 @@
     </row>
     <row r="474" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A474" t="s">
-        <v>518</v>
+        <v>500</v>
       </c>
       <c r="B474">
         <v>9</v>
@@ -68404,7 +68408,7 @@
     </row>
     <row r="475" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A475" t="s">
-        <v>519</v>
+        <v>501</v>
       </c>
       <c r="B475">
         <v>1</v>
@@ -68544,7 +68548,7 @@
     </row>
     <row r="476" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A476" t="s">
-        <v>520</v>
+        <v>502</v>
       </c>
       <c r="B476">
         <v>7</v>
@@ -68684,7 +68688,7 @@
     </row>
     <row r="477" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A477" t="s">
-        <v>521</v>
+        <v>503</v>
       </c>
       <c r="B477">
         <v>6</v>
@@ -68824,7 +68828,7 @@
     </row>
     <row r="478" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A478" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="B478">
         <v>2</v>
@@ -68964,7 +68968,7 @@
     </row>
     <row r="479" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A479" t="s">
-        <v>523</v>
+        <v>505</v>
       </c>
       <c r="B479">
         <v>6</v>
@@ -69104,7 +69108,7 @@
     </row>
     <row r="480" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A480" t="s">
-        <v>524</v>
+        <v>506</v>
       </c>
       <c r="B480">
         <v>9</v>
@@ -69244,7 +69248,7 @@
     </row>
     <row r="481" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A481" t="s">
-        <v>525</v>
+        <v>507</v>
       </c>
       <c r="B481">
         <v>4</v>
@@ -69384,7 +69388,7 @@
     </row>
     <row r="482" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A482" t="s">
-        <v>526</v>
+        <v>508</v>
       </c>
       <c r="B482">
         <v>8</v>
@@ -69524,7 +69528,7 @@
     </row>
     <row r="483" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A483" t="s">
-        <v>527</v>
+        <v>509</v>
       </c>
       <c r="B483">
         <v>5</v>
@@ -69664,7 +69668,7 @@
     </row>
     <row r="484" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A484" t="s">
-        <v>528</v>
+        <v>510</v>
       </c>
       <c r="B484">
         <v>1</v>
@@ -69804,7 +69808,7 @@
     </row>
     <row r="485" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A485" t="s">
-        <v>529</v>
+        <v>511</v>
       </c>
       <c r="B485">
         <v>1</v>
@@ -69944,7 +69948,7 @@
     </row>
     <row r="486" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A486" t="s">
-        <v>530</v>
+        <v>512</v>
       </c>
       <c r="B486">
         <v>4</v>
@@ -70084,7 +70088,7 @@
     </row>
     <row r="487" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A487" t="s">
-        <v>531</v>
+        <v>513</v>
       </c>
       <c r="B487">
         <v>1</v>
@@ -70224,7 +70228,7 @@
     </row>
     <row r="488" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A488" t="s">
-        <v>532</v>
+        <v>514</v>
       </c>
       <c r="B488">
         <v>4</v>
@@ -70364,7 +70368,7 @@
     </row>
     <row r="489" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A489" t="s">
-        <v>533</v>
+        <v>515</v>
       </c>
       <c r="B489">
         <v>6</v>
@@ -70504,7 +70508,7 @@
     </row>
     <row r="490" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A490" t="s">
-        <v>534</v>
+        <v>516</v>
       </c>
       <c r="B490">
         <v>9</v>
@@ -70644,7 +70648,7 @@
     </row>
     <row r="491" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A491" t="s">
-        <v>535</v>
+        <v>517</v>
       </c>
       <c r="B491">
         <v>9</v>
@@ -70784,7 +70788,7 @@
     </row>
     <row r="492" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A492" t="s">
-        <v>536</v>
+        <v>518</v>
       </c>
       <c r="B492">
         <v>2</v>
@@ -70924,7 +70928,7 @@
     </row>
     <row r="493" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A493" t="s">
-        <v>537</v>
+        <v>519</v>
       </c>
       <c r="B493">
         <v>3</v>
@@ -71064,7 +71068,7 @@
     </row>
     <row r="494" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A494" t="s">
-        <v>538</v>
+        <v>520</v>
       </c>
       <c r="B494">
         <v>9</v>
@@ -71204,7 +71208,7 @@
     </row>
     <row r="495" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A495" t="s">
-        <v>539</v>
+        <v>521</v>
       </c>
       <c r="B495">
         <v>6</v>
@@ -71344,7 +71348,7 @@
     </row>
     <row r="496" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A496" t="s">
-        <v>540</v>
+        <v>522</v>
       </c>
       <c r="B496">
         <v>8</v>
@@ -71484,7 +71488,7 @@
     </row>
     <row r="497" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A497" t="s">
-        <v>541</v>
+        <v>523</v>
       </c>
       <c r="B497">
         <v>6</v>
@@ -71624,7 +71628,7 @@
     </row>
     <row r="498" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A498" t="s">
-        <v>542</v>
+        <v>524</v>
       </c>
       <c r="B498">
         <v>2</v>
@@ -71764,7 +71768,7 @@
     </row>
     <row r="499" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A499" t="s">
-        <v>543</v>
+        <v>525</v>
       </c>
       <c r="B499">
         <v>10</v>
@@ -71904,7 +71908,7 @@
     </row>
     <row r="500" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A500" t="s">
-        <v>544</v>
+        <v>526</v>
       </c>
       <c r="B500">
         <v>2</v>
@@ -72044,7 +72048,7 @@
     </row>
     <row r="501" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A501" t="s">
-        <v>545</v>
+        <v>527</v>
       </c>
       <c r="B501">
         <v>3</v>

</xml_diff>